<commit_message>
Removed treatment of MAM
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Tanzania/regions/InputForCode_Arusha.xlsx
+++ b/input_spreadsheets/Tanzania/regions/InputForCode_Arusha.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Tanzania/regions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B0C10D-EAC3-0643-89E0-875757463022}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{66035FD5-0545-3D45-95C3-94EFCA299A7D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="15540" tabRatio="500" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="15540" tabRatio="500" firstSheet="30" activeTab="31" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Expenditure &amp; budget" sheetId="50" r:id="rId1"/>
@@ -64,7 +64,7 @@
     <definedName name="PWPop">'[1]Baseline year demographics'!$C$44:$C$47</definedName>
     <definedName name="WRAPop">'[1]Baseline year demographics'!$C$32:$C$35</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -4165,7 +4165,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1409" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="274">
   <si>
     <t>year</t>
   </si>
@@ -4968,18 +4968,6 @@
     <t>Risk</t>
   </si>
   <si>
-    <t>neonatal mortality</t>
-  </si>
-  <si>
-    <t>infant mortality</t>
-  </si>
-  <si>
-    <t>under 5 mortality</t>
-  </si>
-  <si>
-    <t>maternal mortality</t>
-  </si>
-  <si>
     <t>Available budget</t>
   </si>
   <si>
@@ -4987,6 +4975,18 @@
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>maternal</t>
+  </si>
+  <si>
+    <t>neonatal</t>
+  </si>
+  <si>
+    <t>infant</t>
+  </si>
+  <si>
+    <t>under 5</t>
   </si>
 </sst>
 </file>
@@ -8824,12 +8824,12 @@
         <v>253</v>
       </c>
       <c r="B1" s="154" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" s="154" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B2" s="155">
         <v>329810.39545454545</v>
@@ -8837,7 +8837,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" s="154" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B3" s="153"/>
     </row>
@@ -15018,6 +15018,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
@@ -15028,11 +15033,6 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -17289,8 +17289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="A6" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -17467,7 +17467,7 @@
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="91" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="C22" s="13">
         <v>23</v>
@@ -17475,7 +17475,7 @@
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="91" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="C23" s="13">
         <v>38</v>
@@ -17483,7 +17483,7 @@
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="91" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="C24" s="13">
         <v>56</v>
@@ -27798,8 +27798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DD2B04F-79CD-644E-8CAB-0B99F3DA0979}">
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -28047,9 +28047,7 @@
       <c r="A39" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="B39" s="91" t="s">
-        <v>161</v>
-      </c>
+      <c r="B39" s="91"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
@@ -29397,7 +29395,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated maize fortification coverage, now including IFAS (PW) for all regions
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Tanzania/regions/InputForCode_Arusha.xlsx
+++ b/input_spreadsheets/Tanzania/regions/InputForCode_Arusha.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Tanzania/regions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{66035FD5-0545-3D45-95C3-94EFCA299A7D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{3C0AECE5-59C1-B043-9433-477467FE9DD5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="15540" tabRatio="500" firstSheet="30" activeTab="31" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="15540" tabRatio="500" firstSheet="28" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Expenditure &amp; budget" sheetId="50" r:id="rId1"/>
@@ -4165,7 +4165,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1409" uniqueCount="274">
   <si>
     <t>year</t>
   </si>
@@ -25304,8 +25304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -25407,7 +25407,7 @@
         <v>141</v>
       </c>
       <c r="B7" s="126">
-        <v>0.36</v>
+        <v>0</v>
       </c>
       <c r="C7" s="148">
         <v>0.95</v>
@@ -27798,8 +27798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DD2B04F-79CD-644E-8CAB-0B99F3DA0979}">
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -27970,7 +27970,9 @@
       <c r="A26" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B26" s="91"/>
+      <c r="B26" s="91" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">

</xml_diff>

<commit_message>
Updated IYCF unit costs to sum to national figure
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Tanzania/regions/InputForCode_Arusha.xlsx
+++ b/input_spreadsheets/Tanzania/regions/InputForCode_Arusha.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/input_spreadsheets/Tanzania/regions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{0469E211-30F5-FE48-89DA-C03DC59594FF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{1F26587A-AD8F-EC40-AA6C-D286DCFF8FB4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19260" windowHeight="15540" tabRatio="500" firstSheet="28" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19260" windowHeight="15540" tabRatio="500" firstSheet="13" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Expenditure &amp; budget" sheetId="50" r:id="rId1"/>
@@ -14963,11 +14963,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B33"/>
@@ -14978,6 +14973,11 @@
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -15213,8 +15213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -15329,7 +15329,7 @@
         <v>0.91500000000000004</v>
       </c>
       <c r="D8">
-        <v>10.49</v>
+        <v>3.78</v>
       </c>
       <c r="E8">
         <v>0.05</v>
@@ -15343,8 +15343,9 @@
         <f t="shared" ref="C9:C12" si="0">1.5*0.61</f>
         <v>0.91500000000000004</v>
       </c>
-      <c r="D9">
-        <v>10.49</v>
+      <c r="D9" s="90">
+        <f>10.49/4</f>
+        <v>2.6225000000000001</v>
       </c>
       <c r="E9">
         <v>0.05</v>
@@ -15358,8 +15359,9 @@
         <f t="shared" si="0"/>
         <v>0.91500000000000004</v>
       </c>
-      <c r="D10">
-        <v>10.49</v>
+      <c r="D10" s="90">
+        <f t="shared" ref="D10:D12" si="1">10.49/4</f>
+        <v>2.6225000000000001</v>
       </c>
       <c r="E10">
         <v>0.05</v>
@@ -15373,8 +15375,9 @@
         <f t="shared" si="0"/>
         <v>0.91500000000000004</v>
       </c>
-      <c r="D11">
-        <v>10.49</v>
+      <c r="D11" s="90">
+        <f t="shared" si="1"/>
+        <v>2.6225000000000001</v>
       </c>
       <c r="E11">
         <v>0.05</v>
@@ -15388,8 +15391,9 @@
         <f t="shared" si="0"/>
         <v>0.91500000000000004</v>
       </c>
-      <c r="D12">
-        <v>10.49</v>
+      <c r="D12" s="90">
+        <f t="shared" si="1"/>
+        <v>2.6225000000000001</v>
       </c>
       <c r="E12">
         <v>0.05</v>
@@ -25409,7 +25413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>

</xml_diff>